<commit_message>
Read data from an XL is successful
</commit_message>
<xml_diff>
--- a/src/main/java/com/hotelapp/qa/testdata/testDataInput.xlsx
+++ b/src/main/java/com/hotelapp/qa/testdata/testDataInput.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16065" windowHeight="6405"/>
   </bookViews>
   <sheets>
-    <sheet name="bookingData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="bookingDataOriginal" sheetId="1" r:id="rId1"/>
+    <sheet name="bookingData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="93">
   <si>
     <t>hotelLocation</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Master Card</t>
+  </si>
+  <si>
+    <t>American Express</t>
   </si>
 </sst>
 </file>
@@ -333,9 +339,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,10 +643,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2">
+        <v>43802</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,10 +1389,10 @@
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -697,10 +1429,10 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -709,7 +1441,7 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -750,8 +1482,8 @@
       <c r="L2" s="3">
         <v>1234123445674560</v>
       </c>
-      <c r="M2">
-        <v>4523</v>
+      <c r="M2" s="3">
+        <v>1234</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
@@ -759,8 +1491,8 @@
       <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="P2">
-        <v>2021</v>
+      <c r="P2" s="3">
+        <v>2019</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -800,14 +1532,17 @@
       <c r="L3" s="3">
         <v>1234123445674510</v>
       </c>
-      <c r="M3">
-        <v>4512</v>
+      <c r="M3" s="3">
+        <v>4561</v>
+      </c>
+      <c r="N3" t="s">
+        <v>91</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
       </c>
-      <c r="P3">
-        <v>2023</v>
+      <c r="P3" s="3">
+        <v>2021</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -832,7 +1567,7 @@
       <c r="G4" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I4" t="s">
@@ -847,14 +1582,17 @@
       <c r="L4" s="3">
         <v>1234123445675230</v>
       </c>
-      <c r="M4">
-        <v>4512</v>
+      <c r="M4" s="3">
+        <v>5412</v>
+      </c>
+      <c r="N4" t="s">
+        <v>92</v>
       </c>
       <c r="O4" t="s">
         <v>26</v>
       </c>
-      <c r="P4">
-        <v>2022</v>
+      <c r="P4" s="3">
+        <v>2020</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -894,14 +1632,17 @@
       <c r="L5" s="3">
         <v>1234123445677890</v>
       </c>
-      <c r="M5">
-        <v>6325</v>
+      <c r="M5" s="3">
+        <v>5632</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
       </c>
       <c r="O5" t="s">
         <v>27</v>
       </c>
-      <c r="P5">
-        <v>2021</v>
+      <c r="P5" s="3">
+        <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -941,14 +1682,17 @@
       <c r="L6" s="3">
         <v>1234123445671250</v>
       </c>
-      <c r="M6">
-        <v>5487</v>
+      <c r="M6" s="3">
+        <v>5412</v>
+      </c>
+      <c r="N6" t="s">
+        <v>91</v>
       </c>
       <c r="O6" t="s">
         <v>28</v>
       </c>
-      <c r="P6">
-        <v>2020</v>
+      <c r="P6" s="3">
+        <v>2022</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -973,7 +1717,7 @@
       <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="2">
         <v>43802</v>
       </c>
       <c r="I7" t="s">
@@ -988,14 +1732,17 @@
       <c r="L7" s="3">
         <v>1234123445675120</v>
       </c>
-      <c r="M7">
-        <v>5693</v>
+      <c r="M7" s="3">
+        <v>7854</v>
+      </c>
+      <c r="N7" t="s">
+        <v>92</v>
       </c>
       <c r="O7" t="s">
         <v>29</v>
       </c>
-      <c r="P7">
-        <v>2019</v>
+      <c r="P7" s="3">
+        <v>2021</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1035,14 +1782,17 @@
       <c r="L8" s="3">
         <v>1234123445674510</v>
       </c>
-      <c r="M8">
-        <v>4124</v>
+      <c r="M8" s="3">
+        <v>5656</v>
+      </c>
+      <c r="N8" t="s">
+        <v>23</v>
       </c>
       <c r="O8" t="s">
         <v>30</v>
       </c>
-      <c r="P8">
-        <v>2022</v>
+      <c r="P8" s="3">
+        <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1082,14 +1832,17 @@
       <c r="L9" s="3">
         <v>1234123445677810</v>
       </c>
-      <c r="M9">
-        <v>1147</v>
+      <c r="M9" s="3">
+        <v>7895</v>
+      </c>
+      <c r="N9" t="s">
+        <v>91</v>
       </c>
       <c r="O9" t="s">
         <v>31</v>
       </c>
-      <c r="P9">
-        <v>2021</v>
+      <c r="P9" s="3">
+        <v>2019</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1129,42 +1882,20 @@
       <c r="L10" s="3">
         <v>1234123445670210</v>
       </c>
-      <c r="M10">
-        <v>7788</v>
+      <c r="M10" s="3">
+        <v>1254</v>
+      </c>
+      <c r="N10" t="s">
+        <v>92</v>
       </c>
       <c r="O10" t="s">
         <v>32</v>
       </c>
-      <c r="P10">
-        <v>2023</v>
+      <c r="P10" s="3">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>